<commit_message>
udpated function for survey import
</commit_message>
<xml_diff>
--- a/project1/data/surveyLegend.xlsx
+++ b/project1/data/surveyLegend.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lynig\Desktop\dpsinsights\project1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6C9163B-6975-44A5-A6FA-511CEBEC2CDC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375D5A6B-013C-4A62-ADBF-EA2531879A90}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{044420AF-6D05-47B6-8B41-45B271E5F30D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Less than $25,000</t>
   </si>
@@ -139,6 +139,30 @@
   </si>
   <si>
     <t>Actually paid $0 for all hair cuts</t>
+  </si>
+  <si>
+    <t>11-20</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Asian / Pacific Islander</t>
+  </si>
+  <si>
+    <t>Black or African American</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Facebook</t>
   </si>
 </sst>
 </file>
@@ -224,16 +248,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,42 +574,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70AB46FE-640B-4A54-8682-7460572D0770}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:P98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C16" sqref="C16:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="4"/>
+    <col min="9" max="9" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2">
-        <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -591,43 +617,49 @@
       <c r="F1" s="3">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="4">
+        <v>1</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4">
+      <c r="J1" s="5">
         <v>5</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="5">
+      <c r="L1" s="6">
         <v>7</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="6">
+      <c r="N1" s="7">
         <v>1</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O1">
+      <c r="P1" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
@@ -635,43 +667,49 @@
       <c r="F2" s="3">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="5">
         <v>4</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="5">
+      <c r="L2" s="6">
         <v>6</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="6">
+      <c r="N2" s="7">
         <v>2</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O2">
+      <c r="P2" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>16</v>
@@ -679,32 +717,38 @@
       <c r="F3" s="3">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="4">
+        <v>3</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="5">
         <v>3</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K3" s="6">
         <v>200</v>
       </c>
-      <c r="K3" s="5">
+      <c r="L3" s="6">
         <v>8</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="6">
+      <c r="N3" s="7">
         <v>3</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O3">
+      <c r="P3" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -712,10 +756,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>1</v>
@@ -723,37 +767,43 @@
       <c r="F4" s="3">
         <v>4</v>
       </c>
-      <c r="H4" s="7">
-        <v>43424</v>
-      </c>
-      <c r="I4" s="4">
+      <c r="G4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="4">
+        <v>4</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="5">
         <v>2</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="6">
         <v>5</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="6">
+      <c r="N4" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>26</v>
@@ -761,37 +811,43 @@
       <c r="F5" s="3">
         <v>5</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="4">
+        <v>5</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="5">
         <v>0</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="6">
         <v>4</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="M5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="6">
+      <c r="N5" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>30</v>
@@ -799,26 +855,26 @@
       <c r="F6" s="3">
         <v>8</v>
       </c>
-      <c r="H6" s="4">
+      <c r="I6" s="5">
         <v>10</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="5">
         <v>1</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="6">
         <v>3</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="M6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="6">
+      <c r="N6" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -837,35 +893,37 @@
       <c r="F7" s="3">
         <v>2</v>
       </c>
-      <c r="H7" s="4">
+      <c r="I7" s="5">
         <v>5</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J7" s="5">
         <v>1</v>
       </c>
-      <c r="J7" s="5">
+      <c r="K7" s="6">
         <v>100</v>
       </c>
-      <c r="K7" s="5">
+      <c r="L7" s="6">
         <v>8</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="6">
+      <c r="N7" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>34</v>
@@ -873,25 +931,25 @@
       <c r="F8" s="3">
         <v>4</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="5">
         <v>0</v>
       </c>
-      <c r="I8" s="4">
+      <c r="J8" s="5">
         <v>0</v>
       </c>
-      <c r="J8" s="8">
+      <c r="K8" s="8">
         <v>43424</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L8" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>36</v>
@@ -899,28 +957,473 @@
       <c r="F9" s="3">
         <v>7</v>
       </c>
-      <c r="J9" s="5">
+      <c r="K9" s="6">
         <v>10</v>
       </c>
-      <c r="K9" s="5">
+      <c r="L9" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="5">
+      <c r="L10" s="6">
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="str">
+        <f>"'"&amp;A16&amp;"',"</f>
+        <v>'Walk in',</v>
+      </c>
+      <c r="D16" s="4" t="str">
+        <f>""&amp;B16&amp;","</f>
+        <v>1,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4" t="str">
+        <f t="shared" ref="C17:C23" si="0">"'"&amp;A17&amp;"',"</f>
+        <v>'Referral',</v>
+      </c>
+      <c r="D17" s="4" t="str">
+        <f t="shared" ref="D17:D23" si="1">""&amp;B17&amp;","</f>
+        <v>2,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'Yelp',</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>3,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'Google',</v>
+      </c>
+      <c r="D19" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>4,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'Facebook',</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>6,</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2">
+        <v>5</v>
+      </c>
+      <c r="C21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'other',</v>
+      </c>
+      <c r="D21" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>5,</v>
+      </c>
+      <c r="G21"/>
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2">
+        <v>7</v>
+      </c>
+      <c r="C22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'discovered from driving by',</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>7,</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="2">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>'other',</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>8,</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G24"/>
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G25"/>
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G26"/>
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G27"/>
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G28"/>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G29"/>
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G30"/>
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G31"/>
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G32"/>
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G33"/>
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G34"/>
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G35"/>
+      <c r="H35"/>
+    </row>
+    <row r="36" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G36"/>
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G37"/>
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G38"/>
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G39"/>
+      <c r="H39"/>
+    </row>
+    <row r="40" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G40"/>
+      <c r="H40"/>
+    </row>
+    <row r="41" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G41"/>
+      <c r="H41"/>
+    </row>
+    <row r="42" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G42"/>
+      <c r="H42"/>
+    </row>
+    <row r="43" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G43"/>
+      <c r="H43"/>
+    </row>
+    <row r="44" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G44"/>
+      <c r="H44"/>
+    </row>
+    <row r="45" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G45"/>
+      <c r="H45"/>
+    </row>
+    <row r="46" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G46"/>
+      <c r="H46"/>
+    </row>
+    <row r="47" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G47"/>
+      <c r="H47"/>
+    </row>
+    <row r="48" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G48"/>
+      <c r="H48"/>
+    </row>
+    <row r="49" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G49"/>
+      <c r="H49"/>
+    </row>
+    <row r="50" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G50"/>
+      <c r="H50"/>
+    </row>
+    <row r="51" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G51"/>
+      <c r="H51"/>
+    </row>
+    <row r="52" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G52"/>
+      <c r="H52"/>
+    </row>
+    <row r="53" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G53"/>
+      <c r="H53"/>
+    </row>
+    <row r="54" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G54"/>
+      <c r="H54"/>
+    </row>
+    <row r="55" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G55"/>
+      <c r="H55"/>
+    </row>
+    <row r="56" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G56"/>
+      <c r="H56"/>
+    </row>
+    <row r="57" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G57"/>
+      <c r="H57"/>
+    </row>
+    <row r="58" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G58"/>
+      <c r="H58"/>
+    </row>
+    <row r="59" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G59"/>
+      <c r="H59"/>
+    </row>
+    <row r="60" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G60"/>
+      <c r="H60"/>
+    </row>
+    <row r="61" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G61"/>
+      <c r="H61"/>
+    </row>
+    <row r="62" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G62"/>
+      <c r="H62"/>
+    </row>
+    <row r="63" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G63"/>
+      <c r="H63"/>
+    </row>
+    <row r="64" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G64"/>
+      <c r="H64"/>
+    </row>
+    <row r="65" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G65"/>
+      <c r="H65"/>
+    </row>
+    <row r="66" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G66"/>
+      <c r="H66"/>
+    </row>
+    <row r="67" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G67"/>
+      <c r="H67"/>
+    </row>
+    <row r="68" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G68"/>
+      <c r="H68"/>
+    </row>
+    <row r="69" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G69"/>
+      <c r="H69"/>
+    </row>
+    <row r="70" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G70"/>
+      <c r="H70"/>
+    </row>
+    <row r="71" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G71"/>
+      <c r="H71"/>
+    </row>
+    <row r="72" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G72"/>
+      <c r="H72"/>
+    </row>
+    <row r="73" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G73"/>
+      <c r="H73"/>
+    </row>
+    <row r="74" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G74"/>
+      <c r="H74"/>
+    </row>
+    <row r="75" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G75"/>
+      <c r="H75"/>
+    </row>
+    <row r="76" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G76"/>
+      <c r="H76"/>
+    </row>
+    <row r="77" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G77"/>
+      <c r="H77"/>
+    </row>
+    <row r="78" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G78"/>
+      <c r="H78"/>
+    </row>
+    <row r="79" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G79"/>
+      <c r="H79"/>
+    </row>
+    <row r="80" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G80"/>
+      <c r="H80"/>
+    </row>
+    <row r="81" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G81"/>
+      <c r="H81"/>
+    </row>
+    <row r="82" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G82"/>
+      <c r="H82"/>
+    </row>
+    <row r="83" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G83"/>
+      <c r="H83"/>
+    </row>
+    <row r="84" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G84"/>
+      <c r="H84"/>
+    </row>
+    <row r="85" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G85"/>
+      <c r="H85"/>
+    </row>
+    <row r="86" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G86"/>
+      <c r="H86"/>
+    </row>
+    <row r="87" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G87"/>
+      <c r="H87"/>
+    </row>
+    <row r="88" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G88"/>
+      <c r="H88"/>
+    </row>
+    <row r="89" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G89"/>
+      <c r="H89"/>
+    </row>
+    <row r="90" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G90"/>
+      <c r="H90"/>
+    </row>
+    <row r="91" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G91"/>
+      <c r="H91"/>
+    </row>
+    <row r="92" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G92"/>
+      <c r="H92"/>
+    </row>
+    <row r="93" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G93"/>
+      <c r="H93"/>
+    </row>
+    <row r="94" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G94"/>
+      <c r="H94"/>
+    </row>
+    <row r="95" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G95"/>
+      <c r="H95"/>
+    </row>
+    <row r="96" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G96"/>
+      <c r="H96"/>
+    </row>
+    <row r="97" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G97"/>
+      <c r="H97"/>
+    </row>
+    <row r="98" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G98"/>
+      <c r="H98"/>
+    </row>
   </sheetData>
+  <sortState ref="C1:D8">
+    <sortCondition ref="D1:D8"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>